<commit_message>
rr mié 28 may 2025 19:16:10 CEST
</commit_message>
<xml_diff>
--- a/public/routers/Certificados_de_Ahorro_Energético/Agrario/AGR010_ANEXO_III_DECLARACIÓN_RESPONSABLE_DEL_VALOR_DEL.xlsx
+++ b/public/routers/Certificados_de_Ahorro_Energético/Agrario/AGR010_ANEXO_III_DECLARACIÓN_RESPONSABLE_DEL_VALOR_DEL.xlsx
@@ -436,7 +436,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Velocidad del viento ms</t>
+          <t>Espesor e m</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -456,7 +456,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ciudad</t>
+          <t>Responsable</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -466,7 +466,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dia/s de visita</t>
+          <t>teléfono</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -476,7 +476,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>profesión</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -486,7 +486,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>nif</t>
+          <t>Velocidad del viento ms</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -496,7 +496,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Longitud invernadero m-0</t>
+          <t>nif</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -506,7 +506,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Espesor e m-0</t>
+          <t>dia/s de visita</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -516,7 +516,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Velocidad del viento ms-0</t>
+          <t>Longitud invernadero m-0</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -526,7 +526,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NIF</t>
+          <t>K kWm2 C-0</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -536,7 +536,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>t C-2</t>
+          <t>nombre 1</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -546,7 +546,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>referencia catastral</t>
+          <t>Conductividad térmica A Wm C-0</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -556,7 +556,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>año</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -566,7 +566,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Responsable</t>
+          <t>Firma1</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -576,7 +576,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>teléfono</t>
+          <t>referencia catastral</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -596,7 +596,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Conductividad térmica A Wm C</t>
+          <t>mes</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -606,7 +606,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>K kWm2 C</t>
+          <t>NIF</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -616,7 +616,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Espesor e m</t>
+          <t>t C-2</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -626,7 +626,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Firma1</t>
+          <t>dirección postal</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -636,7 +636,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>dirección postal</t>
+          <t>t C-1</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -646,7 +646,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>mail</t>
+          <t>año</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -656,7 +656,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>K kWm2 C-0</t>
+          <t>K kWm2 C</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -666,7 +666,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>nombre 1</t>
+          <t>Conductividad térmica A Wm C</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -676,7 +676,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mes</t>
+          <t>ciudad</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -686,7 +686,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>profesión</t>
+          <t>Espesor e m-0</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -696,7 +696,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Conductividad térmica A Wm C-0</t>
+          <t>Velocidad del viento ms-0</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -706,7 +706,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>t C-1</t>
+          <t>mail</t>
         </is>
       </c>
       <c r="B29" t="n">

</xml_diff>